<commit_message>
Static map saved to file
</commit_message>
<xml_diff>
--- a/input/Berlin.xlsx
+++ b/input/Berlin.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Очень классная новая квартира. Огромный коридор. Уютный район. Далековато.</t>
   </si>
   <si>
-    <t xml:space="preserve">Gensinger Straße 19 in 10315 Berlin</t>
+    <t xml:space="preserve">Gensinger Straße 19, 10315 Berlin</t>
   </si>
   <si>
     <t xml:space="preserve">Район как Воронежская улица. Гетто. Слишком много детей. Квартира огонь, с подвалом.</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Бухенвальд</t>
   </si>
   <si>
-    <t xml:space="preserve">Ella-Kay-Str. 9</t>
+    <t xml:space="preserve">Ella-Kay-Str. 9, 10405 Berlin</t>
   </si>
   <si>
     <t xml:space="preserve">Пафосная квартира с Игорем</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Кладов, домик у воды, ковры</t>
   </si>
   <si>
-    <t xml:space="preserve">Heylstraße 27 in 10825 Berlin</t>
+    <t xml:space="preserve">Heylstraße 27, 10825 Berlin</t>
   </si>
   <si>
     <t xml:space="preserve">Обычная квартира, но очень хорошая</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Домик рядом с лошадьми, бабка и жребий</t>
   </si>
   <si>
-    <t xml:space="preserve">ThreeD Berlin</t>
+    <t xml:space="preserve">Hartriegelstraße 130, 12439 Berlin</t>
   </si>
   <si>
     <t xml:space="preserve">Новостройка, отличная квартира, окрестности не очень.</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">House Nummer 37, домик на склоне за магазинами</t>
   </si>
   <si>
-    <t xml:space="preserve">Letteallee 75 in 13409 Berlin</t>
+    <t xml:space="preserve">Letteallee 75, 13409 Berlin</t>
   </si>
   <si>
     <t xml:space="preserve">Очень плохая квартира — днище, 1 этаж, отвратительный район</t>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">Большие балконы, детская площадка, 1 и 5 этаж</t>
   </si>
   <si>
-    <t xml:space="preserve">Adalbertstraße 44 in 10997 Berlin-Mitte</t>
+    <t xml:space="preserve">Adalbertstraße 44, 10997 Berlin-Mitte</t>
   </si>
   <si>
     <t xml:space="preserve">Дом рядом с бомжатником. Нет коридора и подвала.</t>
@@ -346,7 +346,7 @@
     <t xml:space="preserve">Blankenburger Str. 29, 13156 Berlin</t>
   </si>
   <si>
-    <t xml:space="preserve">Königstr. 47 B in 14163 Zehlendorf</t>
+    <t xml:space="preserve">Königstr. 47B 14163 Zehlendorf</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -471,10 +471,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -560,11 +556,11 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="64.1"/>
@@ -839,7 +835,7 @@
       <c r="A21" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="4" t="n">
         <v>0.375</v>
       </c>
       <c r="D21" s="2" t="n">
@@ -853,7 +849,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="4" t="n">
@@ -867,7 +863,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="4" t="n">
@@ -884,7 +880,7 @@
       <c r="A24" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="7" t="n">
+      <c r="C24" s="4" t="n">
         <v>0.416666666666667</v>
       </c>
       <c r="D24" s="2" t="n">

</xml_diff>